<commit_message>
formatting task related work in this commit
</commit_message>
<xml_diff>
--- a/Charts.xlsx
+++ b/Charts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\GITHUB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\GITHUB\data-analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E30B7B1-E59A-4D01-B964-413BDDA2DA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1E8F24-6CD5-4455-91B5-B820BCB8B754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2070C730-5ED5-4646-A9A9-31579D7D8E9A}"/>
   </bookViews>
@@ -19,9 +19,6 @@
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$64:$A$67</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$63</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$64:$B$67</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$64:$A$67</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$63</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$64:$B$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -282,17 +279,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFD1D9E0"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color rgb="FFD1D9E0"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FFD1D9E0"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFD1D9E0"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -300,9 +297,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -314,6 +314,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -714,6 +715,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-729D-4BDF-B37A-F671523A482F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -729,6 +735,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-729D-4BDF-B37A-F671523A482F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -744,6 +755,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-729D-4BDF-B37A-F671523A482F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -759,6 +775,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-729D-4BDF-B37A-F671523A482F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1795,6 +1816,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-200C-45AA-9918-BB5630EACABD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1810,6 +1836,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-200C-45AA-9918-BB5630EACABD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1825,6 +1856,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-200C-45AA-9918-BB5630EACABD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1840,6 +1876,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-200C-45AA-9918-BB5630EACABD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1855,6 +1896,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-200C-45AA-9918-BB5630EACABD}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2080,6 +2126,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4A73-47DD-AB6F-BDF9A5139E94}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2095,6 +2146,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4A73-47DD-AB6F-BDF9A5139E94}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2110,6 +2166,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-4A73-47DD-AB6F-BDF9A5139E94}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2125,6 +2186,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-4A73-47DD-AB6F-BDF9A5139E94}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -3225,10 +3291,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3239,7 +3305,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{262FFC4C-1884-4AB6-8240-BD06480D6D75}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>Students</cx:v>
             </cx:txData>
           </cx:tx>
@@ -9595,8 +9661,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4267200" y="15835312"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="4267200" y="15082837"/>
+              <a:ext cx="4572000" cy="2686050"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -10072,7 +10138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6068F488-9E80-4D4B-8100-E313F91228C1}">
   <dimension ref="A1:B124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
       <selection activeCell="A120" sqref="A120:B124"/>
     </sheetView>
   </sheetViews>
@@ -10082,396 +10148,403 @@
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:2" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="4">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="5">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="4">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="5">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="4">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="5">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="4">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B38" s="6"/>
     </row>
-    <row r="39" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+    <row r="39" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B43" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+    <row r="51" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="7">
         <v>0.4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+    <row r="53" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="6">
+      <c r="B53" s="8">
         <v>0.35</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="7">
         <v>0.15</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+    <row r="55" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:2" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+    <row r="63" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+    <row r="65" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B65" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
+    <row r="67" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B67" s="4">
+      <c r="B67" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:2" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="B77" s="6"/>
     </row>
-    <row r="78" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
+    <row r="78" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+    <row r="79" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="4" t="s">
+    <row r="80" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B80" s="5">
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3" t="s">
+    <row r="81" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="4">
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
+    <row r="82" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B82" s="5">
         <v>75</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="50.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:2" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
+    <row r="91" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3">
+    <row r="92" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
         <v>2019</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="4">
+    <row r="93" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
         <v>2020</v>
       </c>
-      <c r="B93" s="4">
+      <c r="B93" s="5">
         <v>560</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3">
+    <row r="94" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
         <v>2021</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="4">
         <v>620</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="4">
+    <row r="95" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
         <v>2022</v>
       </c>
-      <c r="B95" s="4">
+      <c r="B95" s="5">
         <v>690</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="3">
+    <row r="96" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
         <v>2023</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="4">
         <v>760</v>
       </c>
     </row>
@@ -10480,44 +10553,43 @@
         <v>48</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
+    <row r="105" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
+    <row r="106" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B106" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
+    <row r="107" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B107" s="4">
+      <c r="B107" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
+    <row r="108" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
+    <row r="109" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B109" s="4">
+      <c r="B109" s="5">
         <v>15</v>
       </c>
     </row>
@@ -10526,44 +10598,43 @@
         <v>54</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
+    <row r="120" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="3" t="s">
+    <row r="121" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B121" s="5">
+      <c r="B121" s="7">
         <v>0.45</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
+    <row r="122" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B122" s="6">
+      <c r="B122" s="8">
         <v>0.25</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="3" t="s">
+    <row r="123" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B123" s="5">
+      <c r="B123" s="7">
         <v>0.2</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="4" t="s">
+    <row r="124" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B124" s="6">
+      <c r="B124" s="8">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>